<commit_message>
All testing resulst now in one file with different sheet names, updated Boxplot creation
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Local, NoCache" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Server, NoCache" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Server, Cache" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -5444,7 +5445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A124"/>
+  <dimension ref="A1:A269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6074,6 +6075,2657 @@
         <v>3</v>
       </c>
     </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>4.400000005960464</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>2.899999976158142</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>3.700000017881393</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>3.400000005960464</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>3.700000017881393</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>3.100000023841858</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>3.599999994039536</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>3.899999976158142</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>2.599999994039536</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>3.100000023841858</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>4.699999988079071</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>3.100000023841858</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>3.700000017881393</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>4.400000005960464</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>3.100000023841858</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>3.799999982118607</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>3.299999982118607</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>3.699999988079071</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>2.699999988079071</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>3.400000005960464</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>3.399999976158142</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>4.400000005960464</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>3.299999982118607</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>11.29999998211861</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>3.700000017881393</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>2.599999994039536</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>2.899999976158142</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>2.899999976158142</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>3.100000023841858</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>2.799999982118607</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>3.400000005960464</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>2.899999976158142</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>3.199999988079071</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>2.700000017881393</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>3.400000005960464</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>2.899999976158142</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>3.200000017881393</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>3.099999994039536</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>3.300000011920929</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>3.400000005960464</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>2.900000005960464</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>2.800000011920929</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A381"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.7999999821186066</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1.100000023841858</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1.600000023841858</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.800000011920929</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1.200000017881393</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1.400000005960464</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>0.8999999761581421</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>0.699999988079071</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>0.800000011920929</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>0.800000011920929</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>1.300000011920929</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>0.8999999761581421</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>1.100000023841858</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>1.200000017881393</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>0.699999988079071</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>1.400000005960464</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>1.200000017881393</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>1.299999982118607</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>1.100000023841858</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>1.299999982118607</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>0.7000000178813934</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>0.699999988079071</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>1.300000011920929</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>1.400000005960464</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>0.7999999821186066</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>1.300000011920929</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>0.300000011920929</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>0.5999999940395355</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>0.9000000059604645</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>1.099999994039536</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>0.2999999821186066</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>0.800000011920929</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>0.4000000059604645</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>0.3999999761581421</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>1.199999988079071</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
first try of getting network timings
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -9,6 +9,7 @@
     <sheet name="Local, NoCache" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Server, NoCache" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Server, Cache" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Testing Timings" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -8729,4 +8730,3275 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A650"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
full timings extracted and written in excel, queued time still missing
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-24360" yWindow="1845" windowWidth="21600" windowHeight="12105" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="29655" yWindow="2625" windowWidth="21600" windowHeight="12120" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Local, NoCache" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,20 +12,25 @@
     <sheet name="Testing Timings" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -44,12 +49,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -77,12 +97,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -452,7 +475,7 @@
   </sheetPr>
   <dimension ref="A1:A995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A908" workbookViewId="0">
+    <sheetView topLeftCell="A908" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6814,7 +6837,7 @@
   </sheetPr>
   <dimension ref="A1:A381"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8738,7 +8761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A650"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8747,3255 +8770,659 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Stalled</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>DNS Lookup</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Initial Connection</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>SSL</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Request Sent</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Waiting</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.008000000000000007</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.06999999999999995</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.2589999930933118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.08399999999999996</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.278</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.256999977864325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.243</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.07100000000000001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.041</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1900000497698784</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.04899999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.127</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.2209999365732074</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.002000000000000002</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.289</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.05800000000000005</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.151</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.2000001259148121</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n">
         <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.07500000000000007</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.114</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.2990000648424029</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" t="n">
         <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.002999999999999989</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.274</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9729999999999999</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.202000024728477</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.257</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.05399999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9340000000000002</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2280001062899828</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="n">
         <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.002999999999999989</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.06100000000000005</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.334</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.2080000704154372</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.05299999999999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.198</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.2610000083222985</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.04599999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.2539999550208449</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.316</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2769998973235488</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="n">
         <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.002999999999999989</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.271</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.707</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.2029999159276485</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="n">
         <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.479</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.06700000000000006</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.057</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.2180000301450491</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.002999999999999989</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.05099999999999999</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9299999999999999</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.265000038780272</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.05199999999999999</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.035</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.202000024728477</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>2</v>
       </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.05299999999999999</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.011</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.1979999942705035</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.257</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.05499999999999999</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9950000000000001</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.2450000029057264</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.002000000000000002</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.259</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.05299999999999999</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.217</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2439998788759112</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.057</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2090000780299306</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
+      <c r="C22" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="F22" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="314">
-      <c r="A314" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="315">
-      <c r="A315" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="316">
-      <c r="A316" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="326">
-      <c r="A326" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="327">
-      <c r="A327" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="363">
-      <c r="A363" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="364">
-      <c r="A364" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="366">
-      <c r="A366" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="367">
-      <c r="A367" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="368">
-      <c r="A368" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="369">
-      <c r="A369" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="370">
-      <c r="A370" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="371">
-      <c r="A371" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="372">
-      <c r="A372" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="373">
-      <c r="A373" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="374">
-      <c r="A374" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="375">
-      <c r="A375" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="376">
-      <c r="A376" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="377">
-      <c r="A377" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="378">
-      <c r="A378" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="379">
-      <c r="A379" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="380">
-      <c r="A380" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="381">
-      <c r="A381" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="382">
-      <c r="A382" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="383">
-      <c r="A383" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="384">
-      <c r="A384" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="385">
-      <c r="A385" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="386">
-      <c r="A386" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="387">
-      <c r="A387" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="388">
-      <c r="A388" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="389">
-      <c r="A389" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="390">
-      <c r="A390" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="391">
-      <c r="A391" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="392">
-      <c r="A392" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="393">
-      <c r="A393" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="394">
-      <c r="A394" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="395">
-      <c r="A395" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="396">
-      <c r="A396" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="397">
-      <c r="A397" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="398">
-      <c r="A398" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="399">
-      <c r="A399" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="400">
-      <c r="A400" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="401">
-      <c r="A401" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="402">
-      <c r="A402" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="403">
-      <c r="A403" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="404">
-      <c r="A404" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="405">
-      <c r="A405" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="406">
-      <c r="A406" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="407">
-      <c r="A407" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="408">
-      <c r="A408" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="409">
-      <c r="A409" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="410">
-      <c r="A410" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="411">
-      <c r="A411" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="412">
-      <c r="A412" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="413">
-      <c r="A413" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="414">
-      <c r="A414" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="415">
-      <c r="A415" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="416">
-      <c r="A416" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="417">
-      <c r="A417" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="418">
-      <c r="A418" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="419">
-      <c r="A419" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="420">
-      <c r="A420" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="421">
-      <c r="A421" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="422">
-      <c r="A422" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="423">
-      <c r="A423" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="424">
-      <c r="A424" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="425">
-      <c r="A425" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="426">
-      <c r="A426" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="427">
-      <c r="A427" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="428">
-      <c r="A428" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="429">
-      <c r="A429" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="430">
-      <c r="A430" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="431">
-      <c r="A431" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="432">
-      <c r="A432" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="433">
-      <c r="A433" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="434">
-      <c r="A434" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="435">
-      <c r="A435" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="436">
-      <c r="A436" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="437">
-      <c r="A437" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="438">
-      <c r="A438" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="439">
-      <c r="A439" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="440">
-      <c r="A440" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="441">
-      <c r="A441" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="442">
-      <c r="A442" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="443">
-      <c r="A443" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="445">
-      <c r="A445" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="446">
-      <c r="A446" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="447">
-      <c r="A447" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="448">
-      <c r="A448" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="449">
-      <c r="A449" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="450">
-      <c r="A450" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="476">
-      <c r="A476" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="477">
-      <c r="A477" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="478">
-      <c r="A478" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="479">
-      <c r="A479" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="480">
-      <c r="A480" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="481">
-      <c r="A481" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="482">
-      <c r="A482" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="483">
-      <c r="A483" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="484">
-      <c r="A484" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="485">
-      <c r="A485" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="486">
-      <c r="A486" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="487">
-      <c r="A487" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="488">
-      <c r="A488" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="489">
-      <c r="A489" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="490">
-      <c r="A490" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="491">
-      <c r="A491" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="492">
-      <c r="A492" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="493">
-      <c r="A493" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="494">
-      <c r="A494" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="495">
-      <c r="A495" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="496">
-      <c r="A496" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="497">
-      <c r="A497" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="498">
-      <c r="A498" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="499">
-      <c r="A499" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="500">
-      <c r="A500" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="501">
-      <c r="A501" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="502">
-      <c r="A502" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="503">
-      <c r="A503" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="504">
-      <c r="A504" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="505">
-      <c r="A505" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="506">
-      <c r="A506" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="507">
-      <c r="A507" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="508">
-      <c r="A508" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="509">
-      <c r="A509" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="510">
-      <c r="A510" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="511">
-      <c r="A511" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="512">
-      <c r="A512" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="513">
-      <c r="A513" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="514">
-      <c r="A514" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="515">
-      <c r="A515" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="516">
-      <c r="A516" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="517">
-      <c r="A517" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="518">
-      <c r="A518" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="519">
-      <c r="A519" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="520">
-      <c r="A520" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="521">
-      <c r="A521" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="522">
-      <c r="A522" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="523">
-      <c r="A523" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="524">
-      <c r="A524" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="525">
-      <c r="A525" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="526">
-      <c r="A526" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="527">
-      <c r="A527" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="528">
-      <c r="A528" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="529">
-      <c r="A529" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="530">
-      <c r="A530" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="531">
-      <c r="A531" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="532">
-      <c r="A532" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="534">
-      <c r="A534" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="535">
-      <c r="A535" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="536">
-      <c r="A536" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="537">
-      <c r="A537" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="538">
-      <c r="A538" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="539">
-      <c r="A539" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="540">
-      <c r="A540" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="541">
-      <c r="A541" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="542">
-      <c r="A542" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="543">
-      <c r="A543" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="544">
-      <c r="A544" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="545">
-      <c r="A545" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="546">
-      <c r="A546" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="547">
-      <c r="A547" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="548">
-      <c r="A548" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="549">
-      <c r="A549" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="550">
-      <c r="A550" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="551">
-      <c r="A551" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="552">
-      <c r="A552" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="553">
-      <c r="A553" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="554">
-      <c r="A554" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="555">
-      <c r="A555" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="556">
-      <c r="A556" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="557">
-      <c r="A557" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="558">
-      <c r="A558" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="559">
-      <c r="A559" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="560">
-      <c r="A560" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="561">
-      <c r="A561" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="562">
-      <c r="A562" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="563">
-      <c r="A563" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="564">
-      <c r="A564" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="565">
-      <c r="A565" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="566">
-      <c r="A566" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="567">
-      <c r="A567" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="568">
-      <c r="A568" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="569">
-      <c r="A569" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="570">
-      <c r="A570" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="571">
-      <c r="A571" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="572">
-      <c r="A572" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="573">
-      <c r="A573" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="574">
-      <c r="A574" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="575">
-      <c r="A575" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="576">
-      <c r="A576" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="577">
-      <c r="A577" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="578">
-      <c r="A578" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="579">
-      <c r="A579" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="580">
-      <c r="A580" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="581">
-      <c r="A581" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="582">
-      <c r="A582" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="583">
-      <c r="A583" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="584">
-      <c r="A584" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="585">
-      <c r="A585" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="586">
-      <c r="A586" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="587">
-      <c r="A587" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="588">
-      <c r="A588" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="589">
-      <c r="A589" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="590">
-      <c r="A590" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="591">
-      <c r="A591" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="592">
-      <c r="A592" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="593">
-      <c r="A593" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="594">
-      <c r="A594" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="595">
-      <c r="A595" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="596">
-      <c r="A596" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="597">
-      <c r="A597" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="598">
-      <c r="A598" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="599">
-      <c r="A599" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="600">
-      <c r="A600" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="601">
-      <c r="A601" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="602">
-      <c r="A602" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="603">
-      <c r="A603" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="604">
-      <c r="A604" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="605">
-      <c r="A605" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="606">
-      <c r="A606" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="607">
-      <c r="A607" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="608">
-      <c r="A608" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="609">
-      <c r="A609" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="610">
-      <c r="A610" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="611">
-      <c r="A611" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="612">
-      <c r="A612" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="613">
-      <c r="A613" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="614">
-      <c r="A614" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="615">
-      <c r="A615" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="616">
-      <c r="A616" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="617">
-      <c r="A617" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="618">
-      <c r="A618" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="619">
-      <c r="A619" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="620">
-      <c r="A620" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="621">
-      <c r="A621" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="622">
-      <c r="A622" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="623">
-      <c r="A623" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="624">
-      <c r="A624" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="625">
-      <c r="A625" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="626">
-      <c r="A626" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="627">
-      <c r="A627" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="628">
-      <c r="A628" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="629">
-      <c r="A629" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="630">
-      <c r="A630" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="631">
-      <c r="A631" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="632">
-      <c r="A632" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="633">
-      <c r="A633" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="634">
-      <c r="A634" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="635">
-      <c r="A635" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="636">
-      <c r="A636" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="637">
-      <c r="A637" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="638">
-      <c r="A638" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="639">
-      <c r="A639" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="640">
-      <c r="A640" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="641">
-      <c r="A641" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="642">
-      <c r="A642" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="643">
-      <c r="A643" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="644">
-      <c r="A644" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="645">
-      <c r="A645" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="646">
-      <c r="A646" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="647">
-      <c r="A647" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="648">
-      <c r="A648" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="649">
-      <c r="A649" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="650">
-      <c r="A650" t="n">
-        <v>2</v>
+      <c r="G22" t="n">
+        <v>0.07300000000000001</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.9059999999999999</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.1949999714270234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy up of unused code, added better input manegment to testing software
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -8761,7 +8761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9425,6 +9425,528 @@
         <v>0.1949999714270234</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3.100000000093132</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.002999999999999947</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.2570000000000001</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.05800000000000005</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.374</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.2440000000660802</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3.400000000023283</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.262</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.04700000000000004</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.2239999998892017</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2.899999999906868</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.06400000000000006</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.072</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.2630000001317967</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3.799999999813735</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.05299999999999994</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.968</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.2409999999599677</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>2.900000000139698</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.262</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.261</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.05800000000000005</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.087</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.2180000001317239</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>2.599999999860302</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.04299999999999998</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.146</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.1859999999851425</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>2.799999999813735</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.04699999999999999</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.151</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.2360000000862783</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3.199999999953434</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.292</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.05700000000000005</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.093</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.2830000000813016</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.07899999999999996</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.114</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.2789999998640269</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3.799999999813735</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.306</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.06400000000000006</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.885</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.2680000000054861</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.274</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.05100000000000005</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.196</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.2379999998538551</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3.199999999953434</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.326</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.05300000000000005</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.227000000222688</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>2.699999999953434</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.05099999999999999</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1.083</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.2269999999953143</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3.099999999860302</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.00399999999999999</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1.461</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.2239999998892017</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>3.100000000093132</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.236</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.05599999999999994</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.113</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.2519999998185085</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.236</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.05599999999999994</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1.113</v>
+      </c>
+      <c r="I39" t="n">
+        <v>44890.77700000007</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1.400000000372529</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.207</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.04400000000000001</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.1800000004550384</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1.299999999813735</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.03900000000000001</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.1400000001012813</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added header to file
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -8761,7 +8761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9947,6 +9947,267 @@
         <v>0.1400000001012813</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>3.200000000186265</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.004999999999999977</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.3110000000000001</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.04899999999999993</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1.291</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.3310000001874869</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>3.299999999813735</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.06099999999999994</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1.284</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.3139999998893472</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.06099999999999994</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.284</v>
+      </c>
+      <c r="I44" t="n">
+        <v>15042.77299999967</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1.800000000279397</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0.3659999997580599</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.155</v>
+      </c>
+      <c r="I46" t="n">
+        <v>14898.16299999984</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>3.700000000186265</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.004999999999999949</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.3770000000000001</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.06900000000000006</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1.365</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.3320000000712753</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.004999999999999949</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.3770000000000001</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.06900000000000006</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1.365</v>
+      </c>
+      <c r="I48" t="n">
+        <v>15033.67400000025</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1.799999999813735</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.218</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.3849999998237763</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.218</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="I50" t="n">
+        <v>15040.71000000022</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
forgot last upload of code comments
</commit_message>
<xml_diff>
--- a/Testing/time_output.xlsx
+++ b/Testing/time_output.xlsx
@@ -1,87 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadim\Desktop\Bach\Testing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8759CE4E-D86A-4730-A3DD-33A36D2AC279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Example times from my Server" sheetId="4" r:id="rId1"/>
+    <sheet name="Example times from my Server" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Testing Timings" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Bust</t>
-  </si>
-  <si>
-    <t>Is Cached</t>
-  </si>
-  <si>
-    <t>Queued</t>
-  </si>
-  <si>
-    <t>Stalled</t>
-  </si>
-  <si>
-    <t>DNS Lookup</t>
-  </si>
-  <si>
-    <t>Initial Connection</t>
-  </si>
-  <si>
-    <t>SSL</t>
-  </si>
-  <si>
-    <t>Request Sent</t>
-  </si>
-  <si>
-    <t>Waiting</t>
-  </si>
-  <si>
-    <t>Download</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,29 +65,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -414,157 +443,434 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col width="29.5703125" customWidth="1" min="7" max="7"/>
+    <col width="13.5703125" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Bust</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Is Cached</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Stalled</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DNS Lookup</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Initial Connection</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SSL</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Request Sent</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Waiting</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>400</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>421</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>99.141199999999998</v>
-      </c>
-      <c r="E2">
-        <v>2.5287099999999998</v>
-      </c>
-      <c r="F2">
+      <c r="D2" t="n">
+        <v>99.1412</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.52871</v>
+      </c>
+      <c r="F2" t="n">
         <v>9.96312</v>
       </c>
-      <c r="G2">
-        <v>52.007021100000003</v>
-      </c>
-      <c r="H2">
-        <v>28.761299999999999</v>
-      </c>
-      <c r="I2">
-        <v>4.9999999999999933E-2</v>
-      </c>
-      <c r="J2">
+      <c r="G2" t="n">
+        <v>52.0070211</v>
+      </c>
+      <c r="H2" t="n">
+        <v>28.7613</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.04999999999999993</v>
+      </c>
+      <c r="J2" t="n">
         <v>25.58173</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="n">
         <v>124.51273</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>81</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="n">
         <v>392</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>79.616399999999999</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="n">
+        <v>79.6164</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.71</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="K3">
-        <v>0.41720000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="B4">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.4172</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="B4" t="n">
         <v>399</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="D4">
-        <v>9.1E-4</v>
-      </c>
-      <c r="E4">
-        <v>5.1000000000000004E-4</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>8.0000000000000007E-5</v>
+      <c r="D4" t="n">
+        <v>0.00091</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.00051</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Bust</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Is Cached</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Stalled</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>DNS Lookup</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Initial Connection</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>SSL</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Request Sent</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Waiting</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3.399999998509884</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.400000002235174</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.005000000000000004</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.284</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.05200000000000005</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.644</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.2539999986765906</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3.099999997764826</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1.400000002235174</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.188</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.005000000000000004</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.04999999999999993</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.322</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.2480000002833549</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.300000000745058</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.314</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.04800000000000004</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.224</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2510000012989622</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3.100000001490116</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.369</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.05599999999999994</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.248</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.2400000012130477</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.199999999254942</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.258</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.186</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.2419999982521404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>